<commit_message>
Agregado a la tabla de decision
</commit_message>
<xml_diff>
--- a/Documentacion/TablaDecision.xlsx
+++ b/Documentacion/TablaDecision.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandro\Desktop\Diseño\TP\2018-jm-group-07\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Facultad\Diseño de Sistemas\Proyectos JAVA\2018-jm-group-07\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CBFC4A-A6A5-4241-AF29-5B0FC432E5A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="18915" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="18915" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Fecha</t>
   </si>
@@ -47,15 +48,6 @@
     <t>Nos permite poder abstraernos de la biblioteca.</t>
   </si>
   <si>
-    <t>Tambien hicimos un wrapper para la clase de JSON Object.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nos permite poner la definicion del formato del JSON en cada clase sin acoplarla a la biblioteca.</t>
-  </si>
-  <si>
-    <t>Nos reduce la probabilidad de errores en el codigo cuando uso el string al hacer por ej comparaciones por mala escritura. Nos obstraemos del string, al directamente utilizar le enumeracion del tipo de documento</t>
-  </si>
-  <si>
     <t>A las categorias residenciales las modelamos como una clase, ya que se comportan todas igual y solo dependen de sus atributos.</t>
   </si>
   <si>
@@ -86,16 +78,40 @@
     <t>Facilita el cálculo del consumo mensual, y además me permite estimar el consumo máximo.</t>
   </si>
   <si>
-    <t>Teniendo en cuenta la decisión de crear una clase para las categorías, decidimos implementar un repositorio, donde se contengan todas las categorías definidas.</t>
-  </si>
-  <si>
     <t>El cliente no necesita conocer los requisitos de cada categoría, ni instanciarlas, sino que simplemente debería saber en qué categoría se debería encontrar y referenciarla a sí mismo.</t>
+  </si>
+  <si>
+    <t>Usar una interfaz de JSON Object. Hacer un wrapper para la clase de JSON Object.</t>
+  </si>
+  <si>
+    <t>Dejamos que la biblioteca se encargue de cómo formatear los JSON.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasar los objetos del dominio al JSONWrapper. </t>
+  </si>
+  <si>
+    <t>Los objetos del dominio están desacoplados de la capa de persistencia del sistema</t>
+  </si>
+  <si>
+    <t>Si en un futuro se le agrega comportamiento, deberíamos crear una clase.</t>
+  </si>
+  <si>
+    <t>Nos reduce la probabilidad de errores en el codigo cuando uso el string al hacer por ej comparaciones por mala escritura. Nos obstraemos del string, al directamente utilizar le enumeracion del tipo de documento.</t>
+  </si>
+  <si>
+    <t>Crear una clase.</t>
+  </si>
+  <si>
+    <t>Es más complejo.</t>
+  </si>
+  <si>
+    <t>Teniendo en cuenta la decisión de crear una clase para las categorías, decidimos implementar un repositorio global, donde se contengan todas las categorías definidas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -167,34 +183,42 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -216,7 +240,8 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -238,8 +263,8 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -261,8 +286,8 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -278,15 +303,14 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -323,13 +347,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E10" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:E10" totalsRowShown="0" dataDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" name="Fecha" dataDxfId="4"/>
-    <tableColumn id="2" name="Decision" dataDxfId="3"/>
-    <tableColumn id="3" name="Ventaja" dataDxfId="2"/>
-    <tableColumn id="4" name="Desventaja" dataDxfId="1"/>
-    <tableColumn id="5" name="Alternativa" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fecha" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Decision" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ventaja" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Desventaja" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Alternativa" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -411,6 +435,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -446,6 +487,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -621,34 +679,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G10:G11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="5" width="13" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="5"/>
+    <col min="2" max="2" width="42.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="5" customWidth="1"/>
+    <col min="4" max="5" width="31.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -662,21 +719,27 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43209</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -685,89 +748,93 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43209</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43209</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>43209</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>43209</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>43212</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>43209</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>43212</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>43209</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>43212</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>43212</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -779,7 +846,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -791,7 +858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Modifico la tabla de decision
</commit_message>
<xml_diff>
--- a/Documentacion/TablaDecision.xlsx
+++ b/Documentacion/TablaDecision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Facultad\Diseño de Sistemas\Proyectos JAVA\2018-jm-group-07\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CBFC4A-A6A5-4241-AF29-5B0FC432E5A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993A5E21-0A2C-478C-8FBB-2D4547B83534}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="18915" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Fecha</t>
   </si>
@@ -45,9 +45,6 @@
     <t xml:space="preserve">Usamos un Adapter/Wrapper para la biblioteca de JSON </t>
   </si>
   <si>
-    <t>Nos permite poder abstraernos de la biblioteca.</t>
-  </si>
-  <si>
     <t>A las categorias residenciales las modelamos como una clase, ya que se comportan todas igual y solo dependen de sus atributos.</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Nos ayuda a que si necesitamos especificar una categoria, directamente la instanciamos con los valores que necesitamos</t>
   </si>
   <si>
-    <t>Nos permite utilizar un tipo de datos nativo de java, que nos ayuda a dominar un requerimiento impuesto para las categorias.Nos garantiza que este en ese rango</t>
-  </si>
-  <si>
     <t>A la clase Cliente le agregamos como atributo una lista de dispositivos.</t>
   </si>
   <si>
@@ -72,15 +66,6 @@
     <t>Utilizamos la interfaz List.</t>
   </si>
   <si>
-    <t>En la estimación del consumo mensual, se tomó en cuenta la cantidad máxima de horas que posee un mes, considerando el consumo máximo de todos los dispositivos que posee el cliente, al ser una estimación.</t>
-  </si>
-  <si>
-    <t>Facilita el cálculo del consumo mensual, y además me permite estimar el consumo máximo.</t>
-  </si>
-  <si>
-    <t>El cliente no necesita conocer los requisitos de cada categoría, ni instanciarlas, sino que simplemente debería saber en qué categoría se debería encontrar y referenciarla a sí mismo.</t>
-  </si>
-  <si>
     <t>Usar una interfaz de JSON Object. Hacer un wrapper para la clase de JSON Object.</t>
   </si>
   <si>
@@ -105,15 +90,113 @@
     <t>Es más complejo.</t>
   </si>
   <si>
-    <t>Teniendo en cuenta la decisión de crear una clase para las categorías, decidimos implementar un repositorio global, donde se contengan todas las categorías definidas.</t>
+    <t>Usamos Service Locator para manejar dependencias de persistencia.</t>
+  </si>
+  <si>
+    <t>Usar directamente un singleton de la dependencia.</t>
+  </si>
+  <si>
+    <t>Agrega complejidad.</t>
+  </si>
+  <si>
+    <t>Reduce el acoplamiento.</t>
+  </si>
+  <si>
+    <t>Hacer una clase por cada categoría residencial.</t>
+  </si>
+  <si>
+    <t>Debemos completar los parámetros cada vez que instanciemos.</t>
+  </si>
+  <si>
+    <t>Utilizar ArrayList o LinkedList.</t>
+  </si>
+  <si>
+    <t>NOTA: LIST FUE IMPUESTO EN EL MAIL</t>
+  </si>
+  <si>
+    <t>Usar dos valores para comparar dentro de un método.</t>
+  </si>
+  <si>
+    <t>Nos permite utilizar un tipo de datos nativo de Java, que nos ayuda a dominar un requerimiento impuesto para las categorias.Nos garantiza que este en ese rango</t>
+  </si>
+  <si>
+    <t>Depender de la implementación de Java.</t>
+  </si>
+  <si>
+    <t>Le asignamos a cada dispositivo la responsabilidad de saber su consumo actual de este mes.</t>
+  </si>
+  <si>
+    <t>Facilita el cálculo del consumo mensual, y además me permite estimar la facturación.</t>
+  </si>
+  <si>
+    <t>Hacer otro tpo de estimación, usando la cantidad máxima que puede consumir el dispositivo en un mes.</t>
+  </si>
+  <si>
+    <t>Es más complejo. Hay que setear el consumo del dispositivo en 0 al principio de cada mes.</t>
+  </si>
+  <si>
+    <t>Teniendo en cuenta la decisión de crear una clase para las categorías residencales, decidimos implementar un repositorio global, donde se contengan todas las categorías residenciales.</t>
+  </si>
+  <si>
+    <t>Logramos que el cliente no necesite conocer los requisitos de cada categoría, ni instanciarlas, sino que simplemente debería saber en qué categoría se debería encontrar y referenciarla a sí mismo.</t>
+  </si>
+  <si>
+    <t>Pasar por parámetro la categoría a la que pertenece y utilizar un ServiceLocator.</t>
+  </si>
+  <si>
+    <t>Acoplamiento entre el cliente y el repositorio de categorías residenciales.</t>
+  </si>
+  <si>
+    <t>Usar directamente la biblioteca de JSON.</t>
+  </si>
+  <si>
+    <t>Nos permite poder abstraernos y desacoplarnos de la biblioteca.</t>
+  </si>
+  <si>
+    <t>No hacer un JSON para los dispositivos, sino que los guardamos en los clientes. El dispositivo solo tiene sentido si pertenece a un  cliente.</t>
+  </si>
+  <si>
+    <t>No hay que hacer un repositorio de dispositivos, no hay que sumar otro archivo.</t>
+  </si>
+  <si>
+    <t>Crear un archivo JSON para los dispositivos y no guardarlos en los clientes.</t>
+  </si>
+  <si>
+    <t>Si en el futuro aparecen dispositivos que no pertenezcan a un cliente o que pertenezcan a más de uno, este esquema no serviría.</t>
+  </si>
+  <si>
+    <t>Crear la interfaz de Almacenamiento Persistencia.</t>
+  </si>
+  <si>
+    <t>El sistema está desacoplado de la implementación de la capa de persistencia.</t>
+  </si>
+  <si>
+    <t>No crear la interfaz y trabajar directamente con el adapter de JSON.</t>
+  </si>
+  <si>
+    <t>Utilizar una lista de tipo dupla integrada por el dispositivo y sus clientes en común.</t>
+  </si>
+  <si>
+    <t>Se ocupa más espacio al tener que crear una lista por cada cliente, además de que puede haber dispositivos repetidos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -175,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,6 +286,21 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -210,14 +308,36 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -263,7 +383,7 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -280,36 +400,14 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -347,13 +445,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:E10" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:E13" totalsRowShown="0" dataDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fecha" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Decision" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ventaja" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Desventaja" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Alternativa" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ventaja" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Desventaja" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Alternativa" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -680,9 +778,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -692,7 +792,7 @@
     <col min="4" max="5" width="31.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -709,7 +809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43209</v>
       </c>
@@ -717,31 +817,33 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43209</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43209</v>
       </c>
@@ -749,92 +851,168 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43209</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>43209</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="C6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
         <v>43209</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>43209</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>43209</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>43212</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>43212</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>43215</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>43215</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>43215</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambios tabla de decision correcio entrega 0
</commit_message>
<xml_diff>
--- a/Documentacion/TablaDecision.xlsx
+++ b/Documentacion/TablaDecision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Facultad\Diseño de Sistemas\Proyectos JAVA\2018-jm-group-07\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993A5E21-0A2C-478C-8FBB-2D4547B83534}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE86CA2-97B0-4023-B64E-F99A92CF9433}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="18915" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>